<commit_message>
updated results file and added tester 3 file
</commit_message>
<xml_diff>
--- a/Wk 8 Submission/Test Results.xlsx
+++ b/Wk 8 Submission/Test Results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmony.sullivan\Desktop\ssw-567-git\ssw567-group5\Wk 8 Submission\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="0" windowWidth="23280" windowHeight="15460" tabRatio="891" activeTab="7"/>
+    <workbookView xWindow="2325" yWindow="0" windowWidth="23280" windowHeight="15465" tabRatio="891"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-Test" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>Pre-Test Questionnaire</t>
   </si>
@@ -164,6 +169,63 @@
   </si>
   <si>
     <t>Easy to get email</t>
+  </si>
+  <si>
+    <t>Chemical Engineer</t>
+  </si>
+  <si>
+    <t>Y/10</t>
+  </si>
+  <si>
+    <t>MS Windows 8 / Laptop</t>
+  </si>
+  <si>
+    <t>2 clicks, 45 seconds</t>
+  </si>
+  <si>
+    <t>Results: Al Safir</t>
+  </si>
+  <si>
+    <t>2 clicks, 29 seconds</t>
+  </si>
+  <si>
+    <t>10+</t>
+  </si>
+  <si>
+    <t>5 minutes 12 seconds</t>
+  </si>
+  <si>
+    <t>Notes: Wasn’t clear how to adjust route options on google maps</t>
+  </si>
+  <si>
+    <t>15+</t>
+  </si>
+  <si>
+    <t>4 minutes 42 seconds</t>
+  </si>
+  <si>
+    <t>Mapquest gave options to tailor route to avoid highways</t>
+  </si>
+  <si>
+    <t>2 minutes 40 seconds</t>
+  </si>
+  <si>
+    <t>1 minute 20 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide information to indicate accuracy of search result
+- e.g. is recommended restaurant Egyptian or Middle Eastern
+- Make options in google maps for tailoring route more easily accessible/configurable.  
+</t>
+  </si>
+  <si>
+    <t>Simple interface for all searches</t>
+  </si>
+  <si>
+    <t>Indicate accuracy of results; eliminate banner/pop-up ads</t>
+  </si>
+  <si>
+    <t>Directory options (e.g. autos, finance, travel, etc.) were a useful alternative to simple searching by text entry field.</t>
   </si>
 </sst>
 </file>
@@ -219,7 +281,7 @@
       <name val="Tahoma"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +413,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -362,22 +430,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,6 +446,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -428,6 +509,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -755,26 +844,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="5" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -786,19 +875,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -808,9 +899,11 @@
       <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="43" thickBot="1">
+      <c r="D4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -818,9 +911,11 @@
       <c r="C5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1">
+      <c r="D5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -830,21 +925,23 @@
       <c r="C6" s="1">
         <v>18</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="D6" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="20" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1">
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -854,9 +951,11 @@
       <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="43" thickBot="1">
+      <c r="D8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -866,9 +965,11 @@
       <c r="C9" s="1">
         <v>3</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="29" thickBot="1">
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -878,9 +979,11 @@
       <c r="C10" s="1">
         <v>10</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="29" thickBot="1">
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -890,7 +993,9 @@
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -908,120 +1013,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
         <v>5</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" thickBot="1">
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="29" thickBot="1">
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" thickBot="1">
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>5</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" thickBot="1">
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
         <v>5</v>
       </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1">
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1039,120 +1166,137 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" thickBot="1">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
         <v>5</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" thickBot="1">
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="43" thickBot="1">
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="43" thickBot="1">
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
-        <v>2</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
         <v>5</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
         <v>5</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" thickBot="1">
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
         <v>5</v>
       </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="29" thickBot="1">
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1170,120 +1314,142 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" thickBot="1">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>3</v>
       </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" thickBot="1">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="43" thickBot="1">
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
-        <v>2</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" thickBot="1">
+      <c r="D5" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
-        <v>2</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="C6" s="7">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" thickBot="1">
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="29" thickBot="1">
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1301,120 +1467,142 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" thickBot="1">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>3</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" thickBot="1">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="43" thickBot="1">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" thickBot="1">
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>5</v>
       </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
-        <v>2</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" thickBot="1">
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="29" thickBot="1">
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1432,120 +1620,137 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" thickBot="1">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" thickBot="1">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="29" thickBot="1">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" thickBot="1">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" thickBot="1">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="29" thickBot="1">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1563,120 +1768,137 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>3</v>
       </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="29" thickBot="1">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="29" thickBot="1">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" thickBot="1">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="29" thickBot="1">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1696,109 +1918,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.5" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" thickBot="1">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="9">
-        <v>2</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1">
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="189.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="14" t="s">
+      <c r="D7" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1819,108 +2053,120 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" thickBot="1">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>5</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>5</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="29" thickBot="1">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="29" thickBot="1">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1">
-      <c r="A8" s="14" t="s">
+      <c r="D7" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>